<commit_message>
refactored code to maintain section
</commit_message>
<xml_diff>
--- a/documents/intents.xlsx
+++ b/documents/intents.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="177">
   <si>
     <t>Intent</t>
   </si>
@@ -555,13 +555,19 @@
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/JavaScript/Reference/Strict_mode</t>
+  </si>
+  <si>
+    <t>basic_global_objects</t>
+  </si>
+  <si>
+    <t>https://wiki.developer.mozilla.org/en-US/docs/Web/JavaScript/Reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,13 +596,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -698,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -712,9 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -736,6 +750,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1030,8 +1053,8 @@
   <dimension ref="A1:G264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,60 +1069,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1115,12 +1138,12 @@
         <v>36</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1132,12 +1155,12 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1149,12 +1172,12 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1166,12 +1189,12 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1183,12 +1206,12 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1200,7 +1223,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1217,7 +1240,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1234,7 +1257,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1253,7 +1276,7 @@
       <c r="F12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1270,7 +1293,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1287,7 +1310,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1306,7 +1329,7 @@
       <c r="F15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1323,7 +1346,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1340,7 +1363,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1357,7 +1380,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1374,7 +1397,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1391,7 +1414,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1408,7 +1431,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1440,7 +1463,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1472,7 +1495,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1489,12 +1512,12 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="15">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1508,7 +1531,7 @@
       <c r="F27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1525,7 +1548,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1542,7 +1565,7 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1561,7 +1584,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="15">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1573,7 +1596,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1590,7 +1613,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1607,12 +1630,12 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="15">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1624,7 +1647,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1641,7 +1664,7 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1658,7 +1681,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1675,7 +1698,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="13" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1692,7 +1715,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1709,7 +1732,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="13" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1726,7 +1749,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1743,7 +1766,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1760,7 +1783,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="13" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1777,7 +1800,7 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="13" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1794,7 +1817,7 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1811,7 +1834,7 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="13" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1828,7 +1851,7 @@
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1845,18 +1868,26 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+    <row r="48" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="4"/>
+      <c r="G48" s="13" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -2858,9 +2889,10 @@
     <hyperlink ref="G45" r:id="rId39" location="Multi-line_template_literals"/>
     <hyperlink ref="G46" r:id="rId40" location="Internationalization"/>
     <hyperlink ref="G47" r:id="rId41"/>
+    <hyperlink ref="G48" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -2900,36 +2932,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2946,7 +2978,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2963,7 +2995,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2980,7 +3012,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2997,7 +3029,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3014,7 +3046,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3031,7 +3063,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3048,7 +3080,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3065,7 +3097,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3082,7 +3114,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3099,7 +3131,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3116,7 +3148,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3133,7 +3165,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3150,7 +3182,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3167,7 +3199,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3184,7 +3216,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3201,7 +3233,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3218,7 +3250,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3235,7 +3267,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3252,7 +3284,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3269,7 +3301,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3286,7 +3318,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3303,7 +3335,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3320,7 +3352,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3337,7 +3369,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="12" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3354,7 +3386,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3371,7 +3403,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3388,7 +3420,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="12" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3405,7 +3437,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3422,7 +3454,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="12" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3439,7 +3471,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="12" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3456,7 +3488,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="12" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4127,36 +4159,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5087,36 +5119,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6033,36 +6065,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -6979,36 +7011,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -7940,36 +7972,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -8890,36 +8922,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>